<commit_message>
Added construction library and updated osm files.
</commit_message>
<xml_diff>
--- a/lib/btap/measures/btap_apply_necb_rules/regional_fuel_type_defaults.xlsx
+++ b/lib/btap/measures/btap_apply_necb_rules/regional_fuel_type_defaults.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="113">
   <si>
     <t>Province</t>
   </si>
@@ -294,15 +294,6 @@
     <t xml:space="preserve">  Resolute_NU_CAN</t>
   </si>
   <si>
-    <t>Dominant Heating FuelType</t>
-  </si>
-  <si>
-    <t>Has MAU?</t>
-  </si>
-  <si>
-    <t>MAU_Heating_Coil_Type</t>
-  </si>
-  <si>
     <t>mau_cooling_type</t>
   </si>
   <si>
@@ -312,12 +303,6 @@
     <t>heating_coil_type_sys_3</t>
   </si>
   <si>
-    <t xml:space="preserve">heating_coil_types_sys4and6 </t>
-  </si>
-  <si>
-    <t>fan_types</t>
-  </si>
-  <si>
     <t>Electricity</t>
   </si>
   <si>
@@ -330,9 +315,6 @@
     <t>Scroll</t>
   </si>
   <si>
-    <t>var_speed_drives</t>
-  </si>
-  <si>
     <t>Natural Gas</t>
   </si>
   <si>
@@ -352,6 +334,27 @@
   </si>
   <si>
     <t>Location</t>
+  </si>
+  <si>
+    <t>boiler_fueltype</t>
+  </si>
+  <si>
+    <t>mau_type</t>
+  </si>
+  <si>
+    <t>mau_heating_coil_type</t>
+  </si>
+  <si>
+    <t>baseboard_type</t>
+  </si>
+  <si>
+    <t>fan_type</t>
+  </si>
+  <si>
+    <t>heating_coil_type_sys4and6</t>
+  </si>
+  <si>
+    <t>var_speed_drive</t>
   </si>
 </sst>
 </file>
@@ -717,10 +720,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U81"/>
+  <dimension ref="A1:V81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="D43" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2:K81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -728,49 +731,53 @@
     <col min="1" max="1" width="31.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="26.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>98</v>
-      </c>
       <c r="J1" s="5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -778,31 +785,34 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D2" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E2" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
@@ -810,31 +820,34 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D3" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E3" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -842,31 +855,34 @@
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D4" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E4" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -874,31 +890,34 @@
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D5" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E5" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
@@ -906,31 +925,34 @@
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D6" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E6" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
@@ -938,31 +960,34 @@
         <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D7" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E7" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
@@ -970,31 +995,34 @@
         <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D8" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E8" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>22</v>
       </c>
@@ -1002,31 +1030,34 @@
         <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D9" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E9" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
@@ -1034,31 +1065,34 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D10" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E10" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>23</v>
       </c>
@@ -1066,31 +1100,34 @@
         <v>1</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D11" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E11" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>24</v>
       </c>
@@ -1098,31 +1135,34 @@
         <v>1</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D12" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E12" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>25</v>
       </c>
@@ -1130,31 +1170,34 @@
         <v>1</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D13" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E13" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>26</v>
       </c>
@@ -1162,31 +1205,34 @@
         <v>1</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D14" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E14" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>27</v>
       </c>
@@ -1194,31 +1240,34 @@
         <v>1</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D15" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E15" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>28</v>
       </c>
@@ -1226,31 +1275,34 @@
         <v>1</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D16" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E16" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>29</v>
       </c>
@@ -1258,31 +1310,34 @@
         <v>1</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D17" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E17" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>30</v>
       </c>
@@ -1290,31 +1345,34 @@
         <v>1</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D18" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E18" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>31</v>
       </c>
@@ -1322,31 +1380,34 @@
         <v>1</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D19" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E19" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>32</v>
       </c>
@@ -1354,31 +1415,34 @@
         <v>1</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D20" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E20" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>33</v>
       </c>
@@ -1386,31 +1450,34 @@
         <v>1</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D21" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E21" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>34</v>
       </c>
@@ -1418,31 +1485,34 @@
         <v>1</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D22" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E22" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>38</v>
       </c>
@@ -1450,32 +1520,34 @@
         <v>2</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="D23" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>101</v>
+        <v>95</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E23" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="K23" s="2"/>
+        <v>96</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="L23" s="2"/>
-      <c r="M23" s="3"/>
+      <c r="M23" s="2"/>
       <c r="N23" s="3"/>
       <c r="O23" s="3"/>
       <c r="P23" s="3"/>
@@ -1484,8 +1556,9 @@
       <c r="S23" s="3"/>
       <c r="T23" s="3"/>
       <c r="U23" s="3"/>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V23" s="3"/>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>39</v>
       </c>
@@ -1493,32 +1566,34 @@
         <v>2</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="D24" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>101</v>
+        <v>95</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E24" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="K24" s="2"/>
+        <v>96</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="L24" s="2"/>
-      <c r="M24" s="3"/>
+      <c r="M24" s="2"/>
       <c r="N24" s="3"/>
       <c r="O24" s="3"/>
       <c r="P24" s="3"/>
@@ -1527,8 +1602,9 @@
       <c r="S24" s="3"/>
       <c r="T24" s="3"/>
       <c r="U24" s="3"/>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V24" s="3"/>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>41</v>
       </c>
@@ -1536,32 +1612,34 @@
         <v>2</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="D25" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>101</v>
+        <v>95</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E25" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="K25" s="2"/>
+        <v>96</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="L25" s="2"/>
-      <c r="M25" s="3"/>
+      <c r="M25" s="2"/>
       <c r="N25" s="3"/>
       <c r="O25" s="3"/>
       <c r="P25" s="3"/>
@@ -1570,8 +1648,9 @@
       <c r="S25" s="3"/>
       <c r="T25" s="3"/>
       <c r="U25" s="3"/>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V25" s="3"/>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>40</v>
       </c>
@@ -1579,32 +1658,34 @@
         <v>2</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="D26" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>101</v>
+        <v>95</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E26" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="K26" s="2"/>
+        <v>96</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="L26" s="2"/>
-      <c r="M26" s="3"/>
+      <c r="M26" s="2"/>
       <c r="N26" s="3"/>
       <c r="O26" s="3"/>
       <c r="P26" s="3"/>
@@ -1613,8 +1694,9 @@
       <c r="S26" s="3"/>
       <c r="T26" s="3"/>
       <c r="U26" s="3"/>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V26" s="3"/>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>42</v>
       </c>
@@ -1622,32 +1704,34 @@
         <v>2</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="D27" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>101</v>
+        <v>95</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E27" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="K27" s="2"/>
+        <v>96</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="L27" s="2"/>
-      <c r="M27" s="3"/>
+      <c r="M27" s="2"/>
       <c r="N27" s="3"/>
       <c r="O27" s="3"/>
       <c r="P27" s="3"/>
@@ -1656,8 +1740,9 @@
       <c r="S27" s="3"/>
       <c r="T27" s="3"/>
       <c r="U27" s="3"/>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V27" s="3"/>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>43</v>
       </c>
@@ -1665,31 +1750,34 @@
         <v>3</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D28" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E28" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>44</v>
       </c>
@@ -1697,31 +1785,34 @@
         <v>3</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D29" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E29" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>45</v>
       </c>
@@ -1729,31 +1820,34 @@
         <v>3</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D30" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E30" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>46</v>
       </c>
@@ -1761,31 +1855,34 @@
         <v>4</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D31" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E31" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>47</v>
       </c>
@@ -1793,31 +1890,34 @@
         <v>4</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D32" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E32" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>15</v>
       </c>
@@ -1825,31 +1925,34 @@
         <v>4</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D33" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E33" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>48</v>
       </c>
@@ -1857,31 +1960,34 @@
         <v>4</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D34" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E34" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>49</v>
       </c>
@@ -1889,31 +1995,34 @@
         <v>4</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D35" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E35" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>50</v>
       </c>
@@ -1921,31 +2030,34 @@
         <v>5</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="D36" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>101</v>
+        <v>95</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E36" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>51</v>
       </c>
@@ -1953,31 +2065,34 @@
         <v>6</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D37" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E37" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="I37" s="4" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>52</v>
       </c>
@@ -1985,31 +2100,34 @@
         <v>6</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D38" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E38" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>53</v>
       </c>
@@ -2017,31 +2135,34 @@
         <v>6</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D39" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E39" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G39" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="I39" s="4" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>57</v>
       </c>
@@ -2049,31 +2170,34 @@
         <v>6</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D40" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E40" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H40" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="I40" s="4" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>35</v>
       </c>
@@ -2081,30 +2205,32 @@
         <v>6</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D41" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E41" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E41" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="I41" s="4" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="M41" s="3"/>
+        <v>101</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="N41" s="3"/>
       <c r="O41" s="3"/>
       <c r="P41" s="3"/>
@@ -2113,8 +2239,9 @@
       <c r="S41" s="3"/>
       <c r="T41" s="3"/>
       <c r="U41" s="3"/>
-    </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V41" s="3"/>
+    </row>
+    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>61</v>
       </c>
@@ -2122,31 +2249,34 @@
         <v>6</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D42" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E42" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E42" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="I42" s="4" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>58</v>
       </c>
@@ -2154,31 +2284,34 @@
         <v>6</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D43" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E43" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E43" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="I43" s="4" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>59</v>
       </c>
@@ -2186,31 +2319,34 @@
         <v>6</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D44" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E44" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E44" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="K44" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>56</v>
       </c>
@@ -2218,30 +2354,32 @@
         <v>6</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D45" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E45" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E45" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G45" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="I45" s="4" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="M45" s="3"/>
+        <v>101</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="N45" s="3"/>
       <c r="O45" s="3"/>
       <c r="P45" s="3"/>
@@ -2250,8 +2388,9 @@
       <c r="S45" s="3"/>
       <c r="T45" s="3"/>
       <c r="U45" s="3"/>
-    </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V45" s="3"/>
+    </row>
+    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>55</v>
       </c>
@@ -2259,30 +2398,32 @@
         <v>6</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D46" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E46" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E46" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="F46" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="I46" s="4" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="J46" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="M46" s="3"/>
+        <v>101</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="N46" s="3"/>
       <c r="O46" s="3"/>
       <c r="P46" s="3"/>
@@ -2291,8 +2432,9 @@
       <c r="S46" s="3"/>
       <c r="T46" s="3"/>
       <c r="U46" s="3"/>
-    </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V46" s="3"/>
+    </row>
+    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>54</v>
       </c>
@@ -2300,30 +2442,32 @@
         <v>6</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D47" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E47" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E47" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="F47" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H47" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="I47" s="4" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="M47" s="3"/>
+        <v>101</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="N47" s="3"/>
       <c r="O47" s="3"/>
       <c r="P47" s="3"/>
@@ -2332,8 +2476,9 @@
       <c r="S47" s="3"/>
       <c r="T47" s="3"/>
       <c r="U47" s="3"/>
-    </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V47" s="3"/>
+    </row>
+    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>36</v>
       </c>
@@ -2341,30 +2486,32 @@
         <v>6</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D48" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E48" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E48" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H48" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="I48" s="4" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="M48" s="3"/>
+        <v>101</v>
+      </c>
+      <c r="K48" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="N48" s="3"/>
       <c r="O48" s="3"/>
       <c r="P48" s="3"/>
@@ -2373,8 +2520,9 @@
       <c r="S48" s="3"/>
       <c r="T48" s="3"/>
       <c r="U48" s="3"/>
-    </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V48" s="3"/>
+    </row>
+    <row r="49" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>60</v>
       </c>
@@ -2382,191 +2530,209 @@
         <v>6</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D49" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E49" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E49" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H49" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="I49" s="4" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D50" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E50" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="K50" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="51" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D51" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E51" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="K51" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="52" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>63</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D52" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E52" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="K52" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="53" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>64</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D53" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E53" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="K53" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="54" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>65</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D54" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E54" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="K54" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="55" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>37</v>
       </c>
@@ -2574,31 +2740,34 @@
         <v>7</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D55" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E55" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E55" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H55" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="I55" s="4" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="J55" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="K55" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="56" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>67</v>
       </c>
@@ -2606,31 +2775,34 @@
         <v>7</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D56" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E56" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E56" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H56" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="I56" s="4" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="J56" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="K56" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="57" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>66</v>
       </c>
@@ -2638,31 +2810,34 @@
         <v>7</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D57" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E57" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E57" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H57" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="I57" s="4" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="J57" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="K57" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="58" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>68</v>
       </c>
@@ -2670,31 +2845,34 @@
         <v>7</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D58" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E58" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E58" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G58" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H58" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="I58" s="4" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="J58" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="K58" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="59" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>69</v>
       </c>
@@ -2702,31 +2880,34 @@
         <v>7</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D59" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E59" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E59" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G59" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H59" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="I59" s="4" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="J59" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="K59" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="60" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>73</v>
       </c>
@@ -2734,30 +2915,32 @@
         <v>8</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D60" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E60" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E60" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G60" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H60" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="I60" s="4" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="J60" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="M60" s="3"/>
+        <v>101</v>
+      </c>
+      <c r="K60" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="N60" s="3"/>
       <c r="O60" s="3"/>
       <c r="P60" s="3"/>
@@ -2766,8 +2949,9 @@
       <c r="S60" s="3"/>
       <c r="T60" s="3"/>
       <c r="U60" s="3"/>
-    </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V60" s="3"/>
+    </row>
+    <row r="61" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>74</v>
       </c>
@@ -2775,30 +2959,32 @@
         <v>8</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D61" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E61" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E61" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G61" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H61" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="I61" s="4" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="J61" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="M61" s="3"/>
+        <v>101</v>
+      </c>
+      <c r="K61" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="N61" s="3"/>
       <c r="O61" s="3"/>
       <c r="P61" s="3"/>
@@ -2807,8 +2993,9 @@
       <c r="S61" s="3"/>
       <c r="T61" s="3"/>
       <c r="U61" s="3"/>
-    </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V61" s="3"/>
+    </row>
+    <row r="62" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>72</v>
       </c>
@@ -2816,30 +3003,32 @@
         <v>8</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D62" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E62" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E62" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G62" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H62" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="I62" s="4" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="J62" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="M62" s="3"/>
+        <v>101</v>
+      </c>
+      <c r="K62" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="N62" s="3"/>
       <c r="O62" s="3"/>
       <c r="P62" s="3"/>
@@ -2848,8 +3037,9 @@
       <c r="S62" s="3"/>
       <c r="T62" s="3"/>
       <c r="U62" s="3"/>
-    </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V62" s="3"/>
+    </row>
+    <row r="63" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>71</v>
       </c>
@@ -2857,31 +3047,34 @@
         <v>8</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D63" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E63" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E63" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G63" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H63" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="I63" s="4" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="J63" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="K63" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="64" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>70</v>
       </c>
@@ -2889,31 +3082,34 @@
         <v>8</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D64" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E64" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E64" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G64" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H64" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="I64" s="4" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="65" spans="1:21" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="K64" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="65" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>75</v>
       </c>
@@ -2921,31 +3117,34 @@
         <v>8</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D65" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E65" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E65" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G65" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H65" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="I65" s="4" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="J65" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="66" spans="1:21" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="K65" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="66" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>76</v>
       </c>
@@ -2953,31 +3152,34 @@
         <v>9</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D66" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E66" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
+      </c>
+      <c r="D66" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E66" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G66" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H66" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="I66" s="4" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="J66" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="67" spans="1:21" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="K66" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="67" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>84</v>
       </c>
@@ -2985,31 +3187,34 @@
         <v>9</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D67" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E67" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E67" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G67" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H67" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="I67" s="4" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="J67" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="68" spans="1:21" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="K67" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="68" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>79</v>
       </c>
@@ -3017,31 +3222,34 @@
         <v>9</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D68" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E68" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E68" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G68" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H68" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="I68" s="4" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="69" spans="1:21" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="K68" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="69" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>78</v>
       </c>
@@ -3049,31 +3257,34 @@
         <v>9</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D69" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E69" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E69" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G69" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H69" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="I69" s="4" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="J69" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="70" spans="1:21" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="K69" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="70" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>77</v>
       </c>
@@ -3081,31 +3292,34 @@
         <v>9</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D70" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E70" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E70" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G70" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H70" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="I70" s="4" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="J70" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="71" spans="1:21" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="K70" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="71" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>82</v>
       </c>
@@ -3113,31 +3327,34 @@
         <v>9</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D71" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E71" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E71" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G71" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H71" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="I71" s="4" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="J71" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="72" spans="1:21" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="K71" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="72" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>80</v>
       </c>
@@ -3145,31 +3362,34 @@
         <v>9</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D72" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E72" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
+      </c>
+      <c r="D72" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E72" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="F72" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G72" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H72" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="I72" s="4" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="J72" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="73" spans="1:21" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="K72" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="73" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>81</v>
       </c>
@@ -3177,31 +3397,34 @@
         <v>9</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D73" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E73" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
+      </c>
+      <c r="D73" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E73" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="F73" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G73" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H73" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="I73" s="4" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="J73" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="74" spans="1:21" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="K73" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="74" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>83</v>
       </c>
@@ -3209,31 +3432,34 @@
         <v>9</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D74" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E74" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
+      </c>
+      <c r="D74" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E74" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="F74" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G74" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H74" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="I74" s="4" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="J74" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="75" spans="1:21" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="K74" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="75" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>86</v>
       </c>
@@ -3241,31 +3467,34 @@
         <v>9</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D75" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E75" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E75" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G75" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H75" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="I75" s="4" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="J75" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="76" spans="1:21" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="K75" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="76" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>87</v>
       </c>
@@ -3273,31 +3502,34 @@
         <v>9</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D76" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E76" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
+      </c>
+      <c r="D76" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E76" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="F76" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G76" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H76" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="I76" s="4" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="J76" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="77" spans="1:21" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="K76" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="77" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>88</v>
       </c>
@@ -3305,31 +3537,34 @@
         <v>9</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D77" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E77" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
+      </c>
+      <c r="D77" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E77" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="F77" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G77" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H77" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="I77" s="4" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="J77" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="78" spans="1:21" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="K77" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="78" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>89</v>
       </c>
@@ -3337,31 +3572,34 @@
         <v>9</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D78" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E78" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
+      </c>
+      <c r="D78" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E78" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="F78" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G78" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H78" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="I78" s="4" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="J78" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="79" spans="1:21" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="K78" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="79" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>85</v>
       </c>
@@ -3369,30 +3607,32 @@
         <v>10</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="D79" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E79" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
+      </c>
+      <c r="D79" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E79" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="F79" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G79" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H79" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I79" s="4" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="J79" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="M79" s="3"/>
+        <v>96</v>
+      </c>
+      <c r="K79" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="N79" s="3"/>
       <c r="O79" s="3"/>
       <c r="P79" s="3"/>
@@ -3401,8 +3641,9 @@
       <c r="S79" s="3"/>
       <c r="T79" s="3"/>
       <c r="U79" s="3"/>
-    </row>
-    <row r="80" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V79" s="3"/>
+    </row>
+    <row r="80" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>90</v>
       </c>
@@ -3410,30 +3651,32 @@
         <v>11</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="D80" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E80" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
+      </c>
+      <c r="D80" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E80" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="F80" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G80" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H80" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I80" s="4" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="J80" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="M80" s="3"/>
+        <v>96</v>
+      </c>
+      <c r="K80" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="N80" s="3"/>
       <c r="O80" s="3"/>
       <c r="P80" s="3"/>
@@ -3442,8 +3685,9 @@
       <c r="S80" s="3"/>
       <c r="T80" s="3"/>
       <c r="U80" s="3"/>
-    </row>
-    <row r="81" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V80" s="3"/>
+    </row>
+    <row r="81" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>91</v>
       </c>
@@ -3451,30 +3695,32 @@
         <v>12</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="D81" s="4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E81" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
+      </c>
+      <c r="D81" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E81" s="4" t="b">
+        <v>1</v>
       </c>
       <c r="F81" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G81" s="4" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="H81" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="I81" s="4" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="J81" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="M81" s="3"/>
+        <v>96</v>
+      </c>
+      <c r="K81" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="N81" s="3"/>
       <c r="O81" s="3"/>
       <c r="P81" s="3"/>
@@ -3483,6 +3729,7 @@
       <c r="S81" s="3"/>
       <c r="T81" s="3"/>
       <c r="U81" s="3"/>
+      <c r="V81" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>